<commit_message>
More functionality added to AHPTree and an example in the scraps section.
</commit_message>
<xml_diff>
--- a/tests/AHPTreeData.xlsx
+++ b/tests/AHPTreeData.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
   <si>
     <t xml:space="preserve">Age</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t xml:space="preserve">A1 vs A3 wrt A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A2 vs A3 wrt A</t>
   </si>
   <si>
     <t xml:space="preserve">B1 vs B2 wrt B</t>
@@ -185,6 +188,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -270,21 +274,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AE8"/>
+  <dimension ref="A1:AF8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="7" style="0" width="17.06"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="17" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="7" style="0" width="17.06"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="18" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -336,7 +340,7 @@
       <c r="Q1" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="0" t="s">
         <v>16</v>
       </c>
       <c r="S1" s="1" t="s">
@@ -378,17 +382,20 @@
       <c r="AE1" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="AF1" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B2" s="0" t="n">
         <f aca="false">RANDBETWEEN(20,50)</f>
         <v>42</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D2" s="0" t="n">
         <f aca="false">RANDBETWEEN(1, 9)^(RANDBETWEEN(0, 1) * 2 -1)</f>
@@ -412,23 +419,27 @@
       </c>
       <c r="I2" s="0" t="n">
         <f aca="false">RANDBETWEEN(1, 9)^(RANDBETWEEN(0, 1) * 2 -1)</f>
+        <v>0.125</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <f aca="false">RANDBETWEEN(1, 9)^(RANDBETWEEN(0, 1) * 2 -1)</f>
         <v>0.2</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="K2" s="0" t="n">
         <f aca="false">RANDBETWEEN(1, 9)^(RANDBETWEEN(0, 1) * 2 -1)</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B3" s="0" t="n">
         <f aca="false">RANDBETWEEN(20,50)</f>
         <v>48</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D3" s="0" t="n">
         <f aca="false">RANDBETWEEN(1, 9)^(RANDBETWEEN(0, 1) * 2 -1)</f>
@@ -452,23 +463,27 @@
       </c>
       <c r="I3" s="0" t="n">
         <f aca="false">RANDBETWEEN(1, 9)^(RANDBETWEEN(0, 1) * 2 -1)</f>
+        <v>1</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <f aca="false">RANDBETWEEN(1, 9)^(RANDBETWEEN(0, 1) * 2 -1)</f>
         <v>0.166666666666667</v>
       </c>
-      <c r="J3" s="0" t="n">
+      <c r="K3" s="0" t="n">
         <f aca="false">RANDBETWEEN(1, 9)^(RANDBETWEEN(0, 1) * 2 -1)</f>
         <v>0.125</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B4" s="0" t="n">
         <f aca="false">RANDBETWEEN(20,50)</f>
         <v>24</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D4" s="0" t="n">
         <f aca="false">RANDBETWEEN(1, 9)^(RANDBETWEEN(0, 1) * 2 -1)</f>
@@ -492,23 +507,27 @@
       </c>
       <c r="I4" s="0" t="n">
         <f aca="false">RANDBETWEEN(1, 9)^(RANDBETWEEN(0, 1) * 2 -1)</f>
+        <v>0.111111111111111</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <f aca="false">RANDBETWEEN(1, 9)^(RANDBETWEEN(0, 1) * 2 -1)</f>
         <v>0.2</v>
       </c>
-      <c r="J4" s="0" t="n">
+      <c r="K4" s="0" t="n">
         <f aca="false">RANDBETWEEN(1, 9)^(RANDBETWEEN(0, 1) * 2 -1)</f>
         <v>0.142857142857143</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B5" s="0" t="n">
         <f aca="false">RANDBETWEEN(20,50)</f>
         <v>38</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">RANDBETWEEN(1, 9)^(RANDBETWEEN(0, 1) * 2 -1)</f>
@@ -532,23 +551,27 @@
       </c>
       <c r="I5" s="0" t="n">
         <f aca="false">RANDBETWEEN(1, 9)^(RANDBETWEEN(0, 1) * 2 -1)</f>
+        <v>1</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <f aca="false">RANDBETWEEN(1, 9)^(RANDBETWEEN(0, 1) * 2 -1)</f>
         <v>3</v>
       </c>
-      <c r="J5" s="0" t="n">
+      <c r="K5" s="0" t="n">
         <f aca="false">RANDBETWEEN(1, 9)^(RANDBETWEEN(0, 1) * 2 -1)</f>
         <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B6" s="0" t="n">
         <f aca="false">RANDBETWEEN(20,50)</f>
         <v>35</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D6" s="0" t="n">
         <f aca="false">RANDBETWEEN(1, 9)^(RANDBETWEEN(0, 1) * 2 -1)</f>
@@ -572,23 +595,27 @@
       </c>
       <c r="I6" s="0" t="n">
         <f aca="false">RANDBETWEEN(1, 9)^(RANDBETWEEN(0, 1) * 2 -1)</f>
+        <v>7</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <f aca="false">RANDBETWEEN(1, 9)^(RANDBETWEEN(0, 1) * 2 -1)</f>
         <v>8</v>
       </c>
-      <c r="J6" s="0" t="n">
+      <c r="K6" s="0" t="n">
         <f aca="false">RANDBETWEEN(1, 9)^(RANDBETWEEN(0, 1) * 2 -1)</f>
         <v>0.111111111111111</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B7" s="0" t="n">
         <f aca="false">RANDBETWEEN(20,50)</f>
         <v>22</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D7" s="0" t="n">
         <f aca="false">RANDBETWEEN(1, 9)^(RANDBETWEEN(0, 1) * 2 -1)</f>
@@ -612,78 +639,82 @@
       </c>
       <c r="I7" s="0" t="n">
         <f aca="false">RANDBETWEEN(1, 9)^(RANDBETWEEN(0, 1) * 2 -1)</f>
+        <v>0.111111111111111</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <f aca="false">RANDBETWEEN(1, 9)^(RANDBETWEEN(0, 1) * 2 -1)</f>
         <v>4</v>
       </c>
-      <c r="J7" s="0" t="n">
+      <c r="K7" s="0" t="n">
         <f aca="false">RANDBETWEEN(1, 9)^(RANDBETWEEN(0, 1) * 2 -1)</f>
         <v>0.333333333333333</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="K8" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="L8" s="0" t="n">
         <v>0.869</v>
       </c>
-      <c r="L8" s="0" t="n">
+      <c r="M8" s="0" t="n">
         <v>0.768</v>
       </c>
-      <c r="M8" s="0" t="n">
+      <c r="N8" s="0" t="n">
         <v>0.143</v>
       </c>
-      <c r="N8" s="0" t="n">
+      <c r="O8" s="0" t="n">
         <v>0.128</v>
       </c>
-      <c r="O8" s="0" t="n">
+      <c r="P8" s="0" t="n">
         <v>0.114</v>
       </c>
-      <c r="P8" s="0" t="n">
+      <c r="Q8" s="0" t="n">
         <v>0.553</v>
       </c>
-      <c r="Q8" s="0" t="n">
+      <c r="R8" s="0" t="n">
         <v>0.391</v>
       </c>
-      <c r="R8" s="0" t="n">
+      <c r="S8" s="0" t="n">
         <v>0.956</v>
       </c>
-      <c r="S8" s="0" t="n">
+      <c r="T8" s="0" t="n">
         <v>0.993</v>
       </c>
-      <c r="T8" s="0" t="n">
+      <c r="U8" s="0" t="n">
         <v>0.906</v>
       </c>
-      <c r="U8" s="0" t="n">
+      <c r="V8" s="0" t="n">
         <v>0.827</v>
       </c>
-      <c r="V8" s="0" t="n">
+      <c r="W8" s="0" t="n">
         <v>0.361</v>
       </c>
-      <c r="W8" s="0" t="n">
+      <c r="X8" s="0" t="n">
         <v>0.66</v>
       </c>
-      <c r="X8" s="0" t="n">
+      <c r="Y8" s="0" t="n">
         <v>0.472</v>
       </c>
-      <c r="Y8" s="0" t="n">
+      <c r="Z8" s="0" t="n">
         <v>0.754</v>
       </c>
-      <c r="Z8" s="0" t="n">
+      <c r="AA8" s="0" t="n">
         <v>0.283</v>
       </c>
-      <c r="AA8" s="0" t="n">
+      <c r="AB8" s="0" t="n">
         <v>0.917</v>
       </c>
-      <c r="AB8" s="0" t="n">
+      <c r="AC8" s="0" t="n">
         <v>0.508</v>
       </c>
-      <c r="AC8" s="0" t="n">
+      <c r="AD8" s="0" t="n">
         <v>0.989</v>
       </c>
-      <c r="AD8" s="0" t="n">
+      <c r="AE8" s="0" t="n">
         <v>0.716</v>
       </c>
-      <c r="AE8" s="0" t="n">
+      <c r="AF8" s="0" t="n">
         <v>0.14</v>
       </c>
     </row>
@@ -716,30 +747,30 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.135</v>
@@ -765,7 +796,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.7</v>
@@ -791,7 +822,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.49</v>
@@ -818,7 +849,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Moving example notebooks around.
</commit_message>
<xml_diff>
--- a/tests/AHPTreeData.xlsx
+++ b/tests/AHPTreeData.xlsx
@@ -140,7 +140,7 @@
     <t xml:space="preserve">Leanne</t>
   </si>
   <si>
-    <t xml:space="preserve">Fireworks</t>
+    <t xml:space="preserve">Blythe</t>
   </si>
   <si>
     <t xml:space="preserve">all</t>
@@ -281,7 +281,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G6" activeCellId="0" sqref="G6"/>
+      <selection pane="bottomRight" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>